<commit_message>
adding workup for excel
</commit_message>
<xml_diff>
--- a/assets/slides/acct3210/S8/AlternativeSavingsVehiclesCalc.xlsx
+++ b/assets/slides/acct3210/S8/AlternativeSavingsVehiclesCalc.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shamussiothrun/ArthurHowardMorris.github.io/assets/slides/acct3210/S8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cahalcaomh/ArthurHowardMorris.github.io/assets/slides/acct3210/S8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D37C2F4-7CCE-6E47-8AB1-36E9016AD050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDB410F0-4D4A-6042-8D6E-9B610D08FDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51240" yWindow="600" windowWidth="25460" windowHeight="42500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33500" windowHeight="21100" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Question 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Question 3 " sheetId="3" r:id="rId2"/>
+    <sheet name="Q1 Step 1" sheetId="5" r:id="rId1"/>
+    <sheet name="Q1 Step2" sheetId="6" r:id="rId2"/>
+    <sheet name="Q1 Step3" sheetId="7" r:id="rId3"/>
+    <sheet name="Q1 Step4" sheetId="8" r:id="rId4"/>
+    <sheet name="Q1 Step5" sheetId="9" r:id="rId5"/>
+    <sheet name="Question 1" sheetId="1" r:id="rId6"/>
+    <sheet name="Question 3 " sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,8 +41,141 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0C6EB82E-0AB9-4244-B9CE-F7D96A60202F}</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{0C6EB82E-0AB9-4244-B9CE-F7D96A60202F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    r(1-t) where r is the yield and t is the tax rate.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Cahal Caomh</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{D4F4CCAB-0A78-6C41-920A-4CCA82294ACB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">r(1-t) where r is the yield and t is the tax rate.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{6EDD0842-A9E5-264A-B377-3440E04EBFE3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">{[(1+R)^n(1−t)+t]^(1/n)} −1 the SPDA annualized return.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Cahal Caomh</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{94088CED-4497-CA4E-AA5D-DA8BDE78EC04}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">r(1-t) where r is the yield and t is the tax rate.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{C9D983B0-6FEB-5E40-8ED3-CCE431409A3E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">{[(1+R)^n(1−t)+t]^(1/n)} −1 the SPDA annualized return.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{52798A67-0BC2-444A-A228-A52857045837}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>replace 't' with 't+.1' to increase the tax rate by the amount of the exise tax</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="31">
   <si>
     <t>Tax-Exempt</t>
   </si>
@@ -124,6 +262,12 @@
   </si>
   <si>
     <t>This is the benefit of the deduction.</t>
+  </si>
+  <si>
+    <t>Rates:</t>
+  </si>
+  <si>
+    <t>Index of Years and Rates</t>
   </si>
 </sst>
 </file>
@@ -133,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,6 +332,19 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -284,7 +441,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,14 +467,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="19" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Comma" xfId="19" builtinId="3"/>
@@ -352,6 +510,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Arthur Morris" id="{90485A80-BBDB-A04D-B9D3-D738207F102C}" userId="S::acarthur@ust.hk::c9c77807-0107-4eef-a133-78b8709f7043" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -674,12 +838,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D3" dT="2024-02-27T09:49:12.62" personId="{90485A80-BBDB-A04D-B9D3-D738207F102C}" id="{0C6EB82E-0AB9-4244-B9CE-F7D96A60202F}">
+    <text>r(1-t) where r is the yield and t is the tax rate.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D8886D-DD2A-4A44-974D-09FA07BA5A68}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,10 +861,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
@@ -714,6 +886,1414 @@
       </c>
       <c r="F3" t="s">
         <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="H5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="H6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="H8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="H9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="H10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="H11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="H12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="H13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="H14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="H15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8DFE8F-611D-1443-8E1B-25088C0A03FA}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="19">
+        <f>$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="H5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19">
+        <f>$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="H6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="19">
+        <f t="shared" ref="C8:C9" si="0">$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="H8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="19">
+        <f t="shared" si="0"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="H9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="H10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="19">
+        <f t="shared" ref="C11:C12" si="1">$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="H11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19">
+        <f t="shared" si="1"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="H12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="H13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="H14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="H15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC6E4FE-D970-4C4E-95C0-004D95035A31}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="19">
+        <f>$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D5" s="19">
+        <f>D$18*(1-$H5)</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="H5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19">
+        <f>$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D6" s="19">
+        <f>D$18*(1-$H6)</f>
+        <v>0.06</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="H6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="19">
+        <f t="shared" ref="C8:C9" si="0">$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D8" s="19">
+        <f t="shared" ref="D7:D15" si="1">D$18*(1-$H8)</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="H8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="19">
+        <f t="shared" si="0"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D9" s="19">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="H9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="H10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="19">
+        <f t="shared" ref="C11:C12" si="2">$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D11" s="19">
+        <f t="shared" si="1"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="H11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19">
+        <f t="shared" si="2"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D12" s="19">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="H12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="H13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D14" s="19">
+        <f t="shared" si="1"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="H14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D15" s="19">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="H15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430F785C-716C-C541-8D5C-ED4B8DD5581C}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="19">
+        <f>$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D5" s="19">
+        <f>D$18*(1-$H5)</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E5" s="19">
+        <f>((1+E$18)^$H4*(1-$H5)+$H5)^(1/$H4)-1</f>
+        <v>6.8253085229591726E-2</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="H5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19">
+        <f>$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D6" s="19">
+        <f>D$18*(1-$H6)</f>
+        <v>0.06</v>
+      </c>
+      <c r="E6" s="19">
+        <f t="shared" ref="E6:E15" si="0">((1+E$18)^$H5*(1-$H6)+$H6)^(1/$H5)-1</f>
+        <v>5.6275013163937571E-2</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="H6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="19">
+        <f t="shared" ref="C8:C9" si="1">$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D8" s="19">
+        <f t="shared" ref="D8:D16" si="2">D$18*(1-$H8)</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E8" s="19">
+        <f t="shared" si="0"/>
+        <v>6.99107855780563E-2</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="H8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="19">
+        <f t="shared" si="1"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D9" s="19">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="E9" s="19">
+        <f t="shared" si="0"/>
+        <v>5.6275013163937571E-2</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="H9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="H10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="19">
+        <f t="shared" ref="C11:C12" si="3">$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D11" s="19">
+        <f t="shared" si="2"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" si="0"/>
+        <v>7.3621759291163436E-2</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="H11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19">
+        <f t="shared" si="3"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D12" s="19">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="E12" s="19">
+        <f t="shared" si="0"/>
+        <v>5.6275013163937571E-2</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="H12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="H13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D14" s="19">
+        <f t="shared" si="2"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E14" s="19">
+        <f t="shared" si="0"/>
+        <v>7.9279124712805515E-2</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="H14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D15" s="19">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="E15" s="19">
+        <f t="shared" si="0"/>
+        <v>5.6275013163937571E-2</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="H15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885C3A85-0387-E148-9F37-B9D9AADDD4FB}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="19">
+        <f>$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D5" s="19">
+        <f>D$18*(1-$H5)</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E5" s="19">
+        <f>((1+E$18)^$H4*(1-$H5)+$H5)^(1/$H4)-1</f>
+        <v>6.8253085229591726E-2</v>
+      </c>
+      <c r="F5" s="19">
+        <f>((1+F$18)^$H4*(1-$H5-0.1)+$H5+0.1)^(1/$H4)-1</f>
+        <v>5.9033004731903205E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19">
+        <f>$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D6" s="19">
+        <f>D$18*(1-$H6)</f>
+        <v>0.06</v>
+      </c>
+      <c r="E6" s="19">
+        <f t="shared" ref="E6:E15" si="0">((1+E$18)^$H5*(1-$H6)+$H6)^(1/$H5)-1</f>
+        <v>5.6275013163937571E-2</v>
+      </c>
+      <c r="F6" s="19">
+        <f t="shared" ref="F6:F15" si="1">((1+F$18)^$H5*(1-$H6-0.1)+$H6+0.1)^(1/$H5)-1</f>
+        <v>4.6745718246369306E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="19">
+        <f t="shared" ref="C8:C9" si="2">$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D8" s="19">
+        <f t="shared" ref="D8:D16" si="3">D$18*(1-$H8)</f>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E8" s="19">
+        <f t="shared" si="0"/>
+        <v>6.99107855780563E-2</v>
+      </c>
+      <c r="F8" s="19">
+        <f t="shared" si="1"/>
+        <v>6.0998952177475196E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="19">
+        <f t="shared" si="2"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D9" s="19">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="E9" s="19">
+        <f t="shared" si="0"/>
+        <v>5.6275013163937571E-2</v>
+      </c>
+      <c r="F9" s="19">
+        <f t="shared" si="1"/>
+        <v>4.6745718246369306E-2</v>
+      </c>
+      <c r="H9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="H10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="19">
+        <f t="shared" ref="C11:C12" si="4">$C$18</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D11" s="19">
+        <f t="shared" si="3"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" si="0"/>
+        <v>7.3621759291163436E-2</v>
+      </c>
+      <c r="F11" s="19">
+        <f t="shared" si="1"/>
+        <v>6.5554653563975496E-2</v>
+      </c>
+      <c r="H11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="19">
+        <f t="shared" si="4"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D12" s="19">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="E12" s="19">
+        <f t="shared" si="0"/>
+        <v>5.6275013163937571E-2</v>
+      </c>
+      <c r="F12" s="19">
+        <f t="shared" si="1"/>
+        <v>4.6745718246369306E-2</v>
+      </c>
+      <c r="H12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="H13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D14" s="19">
+        <f t="shared" si="3"/>
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="E14" s="19">
+        <f t="shared" si="0"/>
+        <v>7.9279124712805515E-2</v>
+      </c>
+      <c r="F14" s="19">
+        <f t="shared" si="1"/>
+        <v>7.2900453889594319E-2</v>
+      </c>
+      <c r="H14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="21">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D15" s="19">
+        <f t="shared" si="3"/>
+        <v>0.06</v>
+      </c>
+      <c r="E15" s="19">
+        <f t="shared" si="0"/>
+        <v>5.6275013163937571E-2</v>
+      </c>
+      <c r="F15" s="19">
+        <f t="shared" si="1"/>
+        <v>4.6745718246369306E-2</v>
+      </c>
+      <c r="H15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -969,6 +2549,9 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
       <c r="C18" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -1003,11 +2586,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDF9EED-0002-6A4F-A5EF-E08FABC666BE}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1091,22 +2674,20 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="16"/>
+      <c r="C7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="20" t="s">
+      <c r="E7" s="16"/>
+      <c r="F7" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="20"/>
+      <c r="A8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">

</xml_diff>